<commit_message>
added DDT tests, constructor and stuff
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\IdeaProjects\selenium2\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761F5001-E123-42B3-A001-C051109AEE4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409F687F-A2C2-48B7-BD97-F7EA845C1238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{5491A8CF-18C5-4385-90CD-2E90B5EA6432}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{5491A8CF-18C5-4385-90CD-2E90B5EA6432}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
+    <sheet name="prime" sheetId="1" r:id="rId1"/>
+    <sheet name="emails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -427,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA289DE-8996-4FF0-8FE2-4FC71A5F7B1A}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -506,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA73639-FC9B-4C36-8697-77760BE0896C}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>